<commit_message>
reworked dist_matrix script to run from main, moving code and functions
</commit_message>
<xml_diff>
--- a/hub_recognition_test_data.xlsx
+++ b/hub_recognition_test_data.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9192297-D3DC-449D-A5BE-55F08023A218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1069,24 +1078,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -1096,7 +1105,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1124,7 +1133,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -1138,77 +1153,67 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1398,20 +1403,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BI31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1:AW1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="47" max="47" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:61" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1610,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:61" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>61</v>
       </c>
@@ -1610,7 +1624,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="7">
-        <v>430.0</v>
+        <v>430</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>65</v>
@@ -1638,10 +1652,10 @@
         <v>72</v>
       </c>
       <c r="O2" s="9">
-        <v>53563.0</v>
+        <v>53563</v>
       </c>
       <c r="P2" s="9">
-        <v>1579.0</v>
+        <v>1579</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>73</v>
@@ -1669,38 +1683,38 @@
       </c>
       <c r="AA2" s="8"/>
       <c r="AB2" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC2" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AD2" s="8"/>
       <c r="AE2" s="8"/>
       <c r="AF2" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AG2" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AH2" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AI2" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AJ2" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AK2" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL2" s="8"/>
       <c r="AM2" s="8"/>
       <c r="AN2" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO2" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AP2" s="11" t="b">
         <v>0</v>
@@ -1726,7 +1740,7 @@
       </c>
       <c r="AX2" s="13"/>
       <c r="AY2" s="9">
-        <v>101814.0</v>
+        <v>101814</v>
       </c>
       <c r="AZ2" s="7" t="s">
         <v>61</v>
@@ -1753,13 +1767,13 @@
         <v>72</v>
       </c>
       <c r="BH2" s="9">
-        <v>53563.0</v>
+        <v>53563</v>
       </c>
       <c r="BI2" s="9">
-        <v>1579.0</v>
+        <v>1579</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:61" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>82</v>
       </c>
@@ -1797,10 +1811,10 @@
         <v>72</v>
       </c>
       <c r="O3" s="9">
-        <v>53511.0</v>
+        <v>53511</v>
       </c>
       <c r="P3" s="9">
-        <v>5509.0</v>
+        <v>5509</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>89</v>
@@ -1828,38 +1842,38 @@
       </c>
       <c r="AA3" s="8"/>
       <c r="AB3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AE3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AF3" s="8"/>
       <c r="AG3" s="8"/>
       <c r="AH3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AI3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AJ3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK3" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL3" s="8"/>
       <c r="AM3" s="8"/>
       <c r="AN3" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP3" s="11" t="b">
         <v>0</v>
@@ -1896,7 +1910,7 @@
       <c r="BH3" s="8"/>
       <c r="BI3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:61" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>91</v>
       </c>
@@ -1910,7 +1924,7 @@
         <v>94</v>
       </c>
       <c r="E4" s="7">
-        <v>605.0</v>
+        <v>605</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
@@ -1934,10 +1948,10 @@
         <v>72</v>
       </c>
       <c r="O4" s="9">
-        <v>53511.0</v>
+        <v>53511</v>
       </c>
       <c r="P4" s="9">
-        <v>3567.0</v>
+        <v>3567</v>
       </c>
       <c r="Q4" s="8" t="s">
         <v>98</v>
@@ -1965,42 +1979,42 @@
       </c>
       <c r="AA4" s="8"/>
       <c r="AB4" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AC4" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AD4" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AE4" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AF4" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AH4" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AI4" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AJ4" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AK4" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AL4" s="8"/>
       <c r="AM4" s="8"/>
       <c r="AN4" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AO4" s="10">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AP4" s="11" t="b">
         <v>0</v>
@@ -2026,7 +2040,7 @@
       </c>
       <c r="AX4" s="13"/>
       <c r="AY4" s="9">
-        <v>14049.0</v>
+        <v>14049</v>
       </c>
       <c r="AZ4" s="7" t="s">
         <v>91</v>
@@ -2053,13 +2067,13 @@
         <v>72</v>
       </c>
       <c r="BH4" s="9">
-        <v>53511.0</v>
+        <v>53511</v>
       </c>
       <c r="BI4" s="9">
-        <v>3567.0</v>
+        <v>3567</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:61" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>101</v>
       </c>
@@ -2097,7 +2111,7 @@
         <v>72</v>
       </c>
       <c r="O5" s="9">
-        <v>53511.0</v>
+        <v>53511</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8" t="s">
@@ -2128,10 +2142,10 @@
       </c>
       <c r="AA5" s="8"/>
       <c r="AB5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD5" s="8"/>
       <c r="AE5" s="8"/>
@@ -2144,10 +2158,10 @@
       <c r="AL5" s="8"/>
       <c r="AM5" s="8"/>
       <c r="AN5" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP5" s="14" t="b">
         <v>1</v>
@@ -2184,7 +2198,7 @@
       <c r="BH5" s="8"/>
       <c r="BI5" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:61" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>111</v>
       </c>
@@ -2222,7 +2236,7 @@
         <v>72</v>
       </c>
       <c r="O6" s="9">
-        <v>53546.0</v>
+        <v>53546</v>
       </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8" t="s">
@@ -2251,10 +2265,10 @@
       </c>
       <c r="AA6" s="8"/>
       <c r="AB6" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
@@ -2267,10 +2281,10 @@
       <c r="AL6" s="8"/>
       <c r="AM6" s="8"/>
       <c r="AN6" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO6" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP6" s="14" t="b">
         <v>1</v>
@@ -2307,7 +2321,7 @@
       <c r="BH6" s="8"/>
       <c r="BI6" s="8"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:61" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>122</v>
       </c>
@@ -2321,7 +2335,7 @@
         <v>94</v>
       </c>
       <c r="E7" s="7">
-        <v>214.0</v>
+        <v>214</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
@@ -2345,10 +2359,10 @@
         <v>72</v>
       </c>
       <c r="O7" s="9">
-        <v>53525.0</v>
+        <v>53525</v>
       </c>
       <c r="P7" s="9">
-        <v>487.0</v>
+        <v>487</v>
       </c>
       <c r="Q7" s="8" t="s">
         <v>128</v>
@@ -2376,42 +2390,42 @@
       </c>
       <c r="AA7" s="8"/>
       <c r="AB7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AC7" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AD7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AF7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AG7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AH7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AI7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AJ7" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8"/>
       <c r="AN7" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO7" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AP7" s="11" t="b">
         <v>0</v>
@@ -2437,7 +2451,7 @@
       </c>
       <c r="AX7" s="13"/>
       <c r="AY7" s="9">
-        <v>14081.0</v>
+        <v>14081</v>
       </c>
       <c r="AZ7" s="7" t="s">
         <v>122</v>
@@ -2464,13 +2478,13 @@
         <v>72</v>
       </c>
       <c r="BH7" s="9">
-        <v>53525.0</v>
+        <v>53525</v>
       </c>
       <c r="BI7" s="9">
-        <v>487.0</v>
+        <v>487</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:61" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>131</v>
       </c>
@@ -2484,7 +2498,7 @@
         <v>94</v>
       </c>
       <c r="E8" s="7">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
@@ -2508,10 +2522,10 @@
         <v>72</v>
       </c>
       <c r="O8" s="9">
-        <v>53534.0</v>
+        <v>53534</v>
       </c>
       <c r="P8" s="9">
-        <v>1836.0</v>
+        <v>1836</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>137</v>
@@ -2539,42 +2553,42 @@
       </c>
       <c r="AA8" s="8"/>
       <c r="AB8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AC8" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AD8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AE8" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AF8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AG8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AH8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AI8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AJ8" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AK8" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8"/>
       <c r="AN8" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AO8" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AP8" s="11" t="b">
         <v>0</v>
@@ -2600,7 +2614,7 @@
       </c>
       <c r="AX8" s="13"/>
       <c r="AY8" s="9">
-        <v>14107.0</v>
+        <v>14107</v>
       </c>
       <c r="AZ8" s="7" t="s">
         <v>131</v>
@@ -2627,13 +2641,13 @@
         <v>72</v>
       </c>
       <c r="BH8" s="9">
-        <v>53534.0</v>
+        <v>53534</v>
       </c>
       <c r="BI8" s="9">
-        <v>1836.0</v>
+        <v>1836</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:61" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>140</v>
       </c>
@@ -2647,7 +2661,7 @@
         <v>94</v>
       </c>
       <c r="E9" s="7">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>143</v>
@@ -2673,10 +2687,10 @@
         <v>72</v>
       </c>
       <c r="O9" s="9">
-        <v>53536.0</v>
+        <v>53536</v>
       </c>
       <c r="P9" s="9">
-        <v>2122.0</v>
+        <v>2122</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>147</v>
@@ -2704,42 +2718,42 @@
       </c>
       <c r="AA9" s="8"/>
       <c r="AB9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AC9" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AD9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AG9" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AH9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AI9" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AJ9" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8"/>
       <c r="AN9" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO9" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AP9" s="11" t="b">
         <v>0</v>
@@ -2765,7 +2779,7 @@
       </c>
       <c r="AX9" s="13"/>
       <c r="AY9" s="9">
-        <v>14115.0</v>
+        <v>14115</v>
       </c>
       <c r="AZ9" s="7" t="s">
         <v>140</v>
@@ -2792,13 +2806,13 @@
         <v>72</v>
       </c>
       <c r="BH9" s="9">
-        <v>53536.0</v>
+        <v>53536</v>
       </c>
       <c r="BI9" s="9">
-        <v>2122.0</v>
+        <v>2122</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:61" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>150</v>
       </c>
@@ -2836,7 +2850,7 @@
         <v>72</v>
       </c>
       <c r="O10" s="9">
-        <v>53536.0</v>
+        <v>53536</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8" t="s">
@@ -2867,10 +2881,10 @@
       </c>
       <c r="AA10" s="8"/>
       <c r="AB10" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC10" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
@@ -2883,10 +2897,10 @@
       <c r="AL10" s="8"/>
       <c r="AM10" s="8"/>
       <c r="AN10" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO10" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP10" s="14" t="b">
         <v>1</v>
@@ -2923,7 +2937,7 @@
       <c r="BH10" s="8"/>
       <c r="BI10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:61" ht="15.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>159</v>
       </c>
@@ -2937,7 +2951,7 @@
         <v>94</v>
       </c>
       <c r="E11" s="7">
-        <v>316.0</v>
+        <v>316</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>116</v>
@@ -2963,10 +2977,10 @@
         <v>72</v>
       </c>
       <c r="O11" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="P11" s="9">
-        <v>3971.0</v>
+        <v>3971</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>163</v>
@@ -2994,42 +3008,42 @@
       </c>
       <c r="AA11" s="8"/>
       <c r="AB11" s="9">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="AC11" s="9">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="AD11" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AE11" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AF11" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AG11" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AH11" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AI11" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AJ11" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AK11" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8"/>
       <c r="AN11" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AO11" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AP11" s="11" t="b">
         <v>0</v>
@@ -3055,7 +3069,7 @@
       </c>
       <c r="AX11" s="13"/>
       <c r="AY11" s="9">
-        <v>14153.0</v>
+        <v>14153</v>
       </c>
       <c r="AZ11" s="7" t="s">
         <v>159</v>
@@ -3082,13 +3096,13 @@
         <v>72</v>
       </c>
       <c r="BH11" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="BI11" s="9">
-        <v>3971.0</v>
+        <v>3971</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:61" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>166</v>
       </c>
@@ -3102,7 +3116,7 @@
         <v>169</v>
       </c>
       <c r="E12" s="7">
-        <v>316.0</v>
+        <v>316</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>116</v>
@@ -3128,10 +3142,10 @@
         <v>72</v>
       </c>
       <c r="O12" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="P12" s="9">
-        <v>3971.0</v>
+        <v>3971</v>
       </c>
       <c r="Q12" s="8" t="s">
         <v>163</v>
@@ -3159,10 +3173,10 @@
       </c>
       <c r="AA12" s="8"/>
       <c r="AB12" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC12" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="8"/>
       <c r="AE12" s="8"/>
@@ -3175,10 +3189,10 @@
       <c r="AL12" s="8"/>
       <c r="AM12" s="8"/>
       <c r="AN12" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO12" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP12" s="14" t="b">
         <v>1</v>
@@ -3204,7 +3218,7 @@
       </c>
       <c r="AX12" s="13"/>
       <c r="AY12" s="9">
-        <v>14153.0</v>
+        <v>14153</v>
       </c>
       <c r="AZ12" s="7" t="s">
         <v>166</v>
@@ -3231,13 +3245,13 @@
         <v>72</v>
       </c>
       <c r="BH12" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="BI12" s="9">
-        <v>3971.0</v>
+        <v>3971</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:61" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>170</v>
       </c>
@@ -3251,7 +3265,7 @@
         <v>169</v>
       </c>
       <c r="E13" s="7">
-        <v>2500.0</v>
+        <v>2500</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7" t="s">
@@ -3277,10 +3291,10 @@
         <v>72</v>
       </c>
       <c r="O13" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="P13" s="9">
-        <v>493.0</v>
+        <v>493</v>
       </c>
       <c r="Q13" s="8" t="s">
         <v>177</v>
@@ -3308,42 +3322,42 @@
       </c>
       <c r="AA13" s="8"/>
       <c r="AB13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AE13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AF13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AG13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AI13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK13" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8"/>
       <c r="AN13" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO13" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP13" s="14" t="b">
         <v>1</v>
@@ -3369,7 +3383,7 @@
       </c>
       <c r="AX13" s="13"/>
       <c r="AY13" s="9">
-        <v>14153.0</v>
+        <v>14153</v>
       </c>
       <c r="AZ13" s="7" t="s">
         <v>170</v>
@@ -3396,13 +3410,13 @@
         <v>72</v>
       </c>
       <c r="BH13" s="9">
-        <v>53545.0</v>
+        <v>53545</v>
       </c>
       <c r="BI13" s="9">
-        <v>493.0</v>
+        <v>493</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:61" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>181</v>
       </c>
@@ -3416,7 +3430,7 @@
         <v>94</v>
       </c>
       <c r="E14" s="7">
-        <v>430.0</v>
+        <v>430</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>65</v>
@@ -3444,10 +3458,10 @@
         <v>72</v>
       </c>
       <c r="O14" s="9">
-        <v>53563.0</v>
+        <v>53563</v>
       </c>
       <c r="P14" s="9">
-        <v>1592.0</v>
+        <v>1592</v>
       </c>
       <c r="Q14" s="8" t="s">
         <v>186</v>
@@ -3475,42 +3489,42 @@
       </c>
       <c r="AA14" s="8"/>
       <c r="AB14" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC14" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AD14" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AE14" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AF14" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AG14" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AH14" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AI14" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AJ14" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AK14" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8"/>
       <c r="AN14" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AO14" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AP14" s="11" t="b">
         <v>0</v>
@@ -3536,7 +3550,7 @@
       </c>
       <c r="AX14" s="13"/>
       <c r="AY14" s="9">
-        <v>14203.0</v>
+        <v>14203</v>
       </c>
       <c r="AZ14" s="7" t="s">
         <v>181</v>
@@ -3563,13 +3577,13 @@
         <v>72</v>
       </c>
       <c r="BH14" s="9">
-        <v>53563.0</v>
+        <v>53563</v>
       </c>
       <c r="BI14" s="9">
-        <v>1592.0</v>
+        <v>1592</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:61" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>189</v>
       </c>
@@ -3583,7 +3597,7 @@
         <v>94</v>
       </c>
       <c r="E15" s="7">
-        <v>519.0</v>
+        <v>519</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>65</v>
@@ -3609,10 +3623,10 @@
         <v>72</v>
       </c>
       <c r="O15" s="9">
-        <v>53576.0</v>
+        <v>53576</v>
       </c>
       <c r="P15" s="9">
-        <v>249.0</v>
+        <v>249</v>
       </c>
       <c r="Q15" s="8" t="s">
         <v>194</v>
@@ -3640,42 +3654,42 @@
       </c>
       <c r="AA15" s="8"/>
       <c r="AB15" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AC15" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AD15" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AF15" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AG15" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AI15" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AJ15" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK15" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AL15" s="8"/>
       <c r="AM15" s="8"/>
       <c r="AN15" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO15" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AP15" s="11" t="b">
         <v>0</v>
@@ -3701,7 +3715,7 @@
       </c>
       <c r="AX15" s="13"/>
       <c r="AY15" s="9">
-        <v>14240.0</v>
+        <v>14240</v>
       </c>
       <c r="AZ15" s="7" t="s">
         <v>189</v>
@@ -3728,13 +3742,13 @@
         <v>72</v>
       </c>
       <c r="BH15" s="9">
-        <v>53576.0</v>
+        <v>53576</v>
       </c>
       <c r="BI15" s="9">
-        <v>249.0</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:61" ht="15.75" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>197</v>
       </c>
@@ -3774,7 +3788,7 @@
         <v>72</v>
       </c>
       <c r="O16" s="9">
-        <v>53576.0</v>
+        <v>53576</v>
       </c>
       <c r="P16" s="8"/>
       <c r="Q16" s="8" t="s">
@@ -3803,10 +3817,10 @@
       </c>
       <c r="AA16" s="8"/>
       <c r="AB16" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AC16" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AD16" s="8"/>
       <c r="AE16" s="8"/>
@@ -3819,10 +3833,10 @@
       <c r="AL16" s="8"/>
       <c r="AM16" s="8"/>
       <c r="AN16" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AO16" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AP16" s="14" t="b">
         <v>1</v>
@@ -3859,7 +3873,7 @@
       <c r="BH16" s="8"/>
       <c r="BI16" s="8"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:61" ht="15.75" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>205</v>
       </c>
@@ -3897,10 +3911,10 @@
         <v>72</v>
       </c>
       <c r="O17" s="9">
-        <v>53103.0</v>
+        <v>53103</v>
       </c>
       <c r="P17" s="9">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="8" t="s">
         <v>212</v>
@@ -3928,42 +3942,42 @@
       </c>
       <c r="AA17" s="8"/>
       <c r="AB17" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AC17" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AD17" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AE17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AF17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AG17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AH17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AI17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AJ17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK17" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8"/>
       <c r="AN17" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AO17" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AP17" s="11" t="b">
         <v>0</v>
@@ -3989,7 +4003,7 @@
       </c>
       <c r="AX17" s="13"/>
       <c r="AY17" s="9">
-        <v>14052.0</v>
+        <v>14052</v>
       </c>
       <c r="AZ17" s="7" t="s">
         <v>205</v>
@@ -4016,13 +4030,13 @@
         <v>72</v>
       </c>
       <c r="BH17" s="9">
-        <v>53103.0</v>
+        <v>53103</v>
       </c>
       <c r="BI17" s="9">
-        <v>40.0</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:61" ht="15.75" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>219</v>
       </c>
@@ -4036,7 +4050,7 @@
         <v>64</v>
       </c>
       <c r="E18" s="7">
-        <v>741.0</v>
+        <v>741</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>221</v>
@@ -4064,10 +4078,10 @@
         <v>72</v>
       </c>
       <c r="O18" s="9">
-        <v>53186.0</v>
+        <v>53186</v>
       </c>
       <c r="P18" s="9">
-        <v>4841.0</v>
+        <v>4841</v>
       </c>
       <c r="Q18" s="8" t="s">
         <v>226</v>
@@ -4095,38 +4109,38 @@
       </c>
       <c r="AA18" s="8"/>
       <c r="AB18" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC18" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AD18" s="8"/>
       <c r="AE18" s="8"/>
       <c r="AF18" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AG18" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AH18" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AI18" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AJ18" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AK18" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AL18" s="8"/>
       <c r="AM18" s="8"/>
       <c r="AN18" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AO18" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AP18" s="11" t="b">
         <v>0</v>
@@ -4156,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="AY18" s="9">
-        <v>101825.0</v>
+        <v>101825</v>
       </c>
       <c r="AZ18" s="7" t="s">
         <v>219</v>
@@ -4183,13 +4197,13 @@
         <v>72</v>
       </c>
       <c r="BH18" s="9">
-        <v>53186.0</v>
+        <v>53186</v>
       </c>
       <c r="BI18" s="9">
-        <v>4841.0</v>
+        <v>4841</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:61" ht="15.75" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>230</v>
       </c>
@@ -4203,7 +4217,7 @@
         <v>94</v>
       </c>
       <c r="E19" s="7">
-        <v>1900.0</v>
+        <v>1900</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>221</v>
@@ -4229,10 +4243,10 @@
         <v>72</v>
       </c>
       <c r="O19" s="9">
-        <v>53005.0</v>
+        <v>53005</v>
       </c>
       <c r="P19" s="9">
-        <v>5097.0</v>
+        <v>5097</v>
       </c>
       <c r="Q19" s="8" t="s">
         <v>237</v>
@@ -4260,42 +4274,42 @@
       </c>
       <c r="AA19" s="8"/>
       <c r="AB19" s="9">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="AC19" s="9">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="AD19" s="9">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="AE19" s="9">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="AF19" s="9">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="AG19" s="9">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="AH19" s="9">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="AI19" s="9">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="AJ19" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AK19" s="9">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="AL19" s="8"/>
       <c r="AM19" s="8"/>
       <c r="AN19" s="10">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="AO19" s="10">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="AP19" s="11" t="b">
         <v>0</v>
@@ -4321,7 +4335,7 @@
       </c>
       <c r="AX19" s="13"/>
       <c r="AY19" s="9">
-        <v>14063.0</v>
+        <v>14063</v>
       </c>
       <c r="AZ19" s="7" t="s">
         <v>230</v>
@@ -4348,13 +4362,13 @@
         <v>72</v>
       </c>
       <c r="BH19" s="9">
-        <v>53005.0</v>
+        <v>53005</v>
       </c>
       <c r="BI19" s="9">
-        <v>5097.0</v>
+        <v>5097</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:61" ht="15.75" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>240</v>
       </c>
@@ -4368,7 +4382,7 @@
         <v>94</v>
       </c>
       <c r="E20" s="7">
-        <v>12808.0</v>
+        <v>12808</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>143</v>
@@ -4394,10 +4408,10 @@
         <v>72</v>
       </c>
       <c r="O20" s="9">
-        <v>53007.0</v>
+        <v>53007</v>
       </c>
       <c r="P20" s="9">
-        <v>1705.0</v>
+        <v>1705</v>
       </c>
       <c r="Q20" s="8" t="s">
         <v>246</v>
@@ -4425,42 +4439,42 @@
       </c>
       <c r="AA20" s="8"/>
       <c r="AB20" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC20" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AD20" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AE20" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AF20" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AG20" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AH20" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AI20" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AJ20" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AK20" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8"/>
       <c r="AN20" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO20" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AP20" s="11" t="b">
         <v>0</v>
@@ -4486,7 +4500,7 @@
       </c>
       <c r="AX20" s="13"/>
       <c r="AY20" s="9">
-        <v>14067.0</v>
+        <v>14067</v>
       </c>
       <c r="AZ20" s="7" t="s">
         <v>240</v>
@@ -4513,13 +4527,13 @@
         <v>72</v>
       </c>
       <c r="BH20" s="9">
-        <v>53007.0</v>
+        <v>53007</v>
       </c>
       <c r="BI20" s="9">
-        <v>1705.0</v>
+        <v>1705</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:61" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>249</v>
       </c>
@@ -4533,7 +4547,7 @@
         <v>94</v>
       </c>
       <c r="E21" s="7">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -4557,10 +4571,10 @@
         <v>72</v>
       </c>
       <c r="O21" s="9">
-        <v>53018.0</v>
+        <v>53018</v>
       </c>
       <c r="P21" s="9">
-        <v>1895.0</v>
+        <v>1895</v>
       </c>
       <c r="Q21" s="8" t="s">
         <v>255</v>
@@ -4588,42 +4602,42 @@
       </c>
       <c r="AA21" s="8"/>
       <c r="AB21" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AC21" s="9">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="AD21" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AE21" s="9">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="AF21" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AG21" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AH21" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AI21" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AJ21" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AK21" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8"/>
       <c r="AN21" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AO21" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AP21" s="11" t="b">
         <v>0</v>
@@ -4649,7 +4663,7 @@
       </c>
       <c r="AX21" s="13"/>
       <c r="AY21" s="9">
-        <v>14098.0</v>
+        <v>14098</v>
       </c>
       <c r="AZ21" s="7" t="s">
         <v>249</v>
@@ -4676,13 +4690,13 @@
         <v>72</v>
       </c>
       <c r="BH21" s="9">
-        <v>53018.0</v>
+        <v>53018</v>
       </c>
       <c r="BI21" s="9">
-        <v>1895.0</v>
+        <v>1895</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:61" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>258</v>
       </c>
@@ -4696,7 +4710,7 @@
         <v>94</v>
       </c>
       <c r="E22" s="7">
-        <v>820.0</v>
+        <v>820</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>65</v>
@@ -4722,10 +4736,10 @@
         <v>72</v>
       </c>
       <c r="O22" s="9">
-        <v>53119.0</v>
+        <v>53119</v>
       </c>
       <c r="P22" s="9">
-        <v>520.0</v>
+        <v>520</v>
       </c>
       <c r="Q22" s="8" t="s">
         <v>263</v>
@@ -4753,42 +4767,42 @@
       </c>
       <c r="AA22" s="8"/>
       <c r="AB22" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC22" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AD22" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AE22" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AF22" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AG22" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AH22" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AI22" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AJ22" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AK22" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="8"/>
       <c r="AM22" s="8"/>
       <c r="AN22" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AO22" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AP22" s="11" t="b">
         <v>0</v>
@@ -4814,7 +4828,7 @@
       </c>
       <c r="AX22" s="13"/>
       <c r="AY22" s="9">
-        <v>14103.0</v>
+        <v>14103</v>
       </c>
       <c r="AZ22" s="7" t="s">
         <v>258</v>
@@ -4841,13 +4855,13 @@
         <v>72</v>
       </c>
       <c r="BH22" s="9">
-        <v>53119.0</v>
+        <v>53119</v>
       </c>
       <c r="BI22" s="9">
-        <v>520.0</v>
+        <v>520</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:61" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>266</v>
       </c>
@@ -4861,7 +4875,7 @@
         <v>94</v>
       </c>
       <c r="E23" s="7">
-        <v>13600.0</v>
+        <v>13600</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
@@ -4885,10 +4899,10 @@
         <v>72</v>
       </c>
       <c r="O23" s="9">
-        <v>53122.0</v>
+        <v>53122</v>
       </c>
       <c r="P23" s="9">
-        <v>1679.0</v>
+        <v>1679</v>
       </c>
       <c r="Q23" s="8" t="s">
         <v>272</v>
@@ -4916,42 +4930,42 @@
       </c>
       <c r="AA23" s="8"/>
       <c r="AB23" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AC23" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AD23" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AE23" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AF23" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AG23" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AH23" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AI23" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AJ23" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AK23" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8"/>
       <c r="AN23" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AO23" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AP23" s="11" t="b">
         <v>0</v>
@@ -4977,7 +4991,7 @@
       </c>
       <c r="AX23" s="13"/>
       <c r="AY23" s="9">
-        <v>14111.0</v>
+        <v>14111</v>
       </c>
       <c r="AZ23" s="7" t="s">
         <v>266</v>
@@ -5004,13 +5018,13 @@
         <v>72</v>
       </c>
       <c r="BH23" s="9">
-        <v>53122.0</v>
+        <v>53122</v>
       </c>
       <c r="BI23" s="9">
-        <v>1679.0</v>
+        <v>1679</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:61" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>275</v>
       </c>
@@ -5024,7 +5038,7 @@
         <v>94</v>
       </c>
       <c r="E24" s="7">
-        <v>209.0</v>
+        <v>209</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
@@ -5048,10 +5062,10 @@
         <v>72</v>
       </c>
       <c r="O24" s="9">
-        <v>53538.0</v>
+        <v>53538</v>
       </c>
       <c r="P24" s="9">
-        <v>2049.0</v>
+        <v>2049</v>
       </c>
       <c r="Q24" s="8" t="s">
         <v>281</v>
@@ -5079,42 +5093,42 @@
       </c>
       <c r="AA24" s="8"/>
       <c r="AB24" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AC24" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AD24" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AE24" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AF24" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AG24" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AH24" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AI24" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AJ24" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AK24" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8"/>
       <c r="AN24" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AO24" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AP24" s="11" t="b">
         <v>0</v>
@@ -5140,7 +5154,7 @@
       </c>
       <c r="AX24" s="13"/>
       <c r="AY24" s="9">
-        <v>14121.0</v>
+        <v>14121</v>
       </c>
       <c r="AZ24" s="7" t="s">
         <v>275</v>
@@ -5167,13 +5181,13 @@
         <v>72</v>
       </c>
       <c r="BH24" s="9">
-        <v>53538.0</v>
+        <v>53538</v>
       </c>
       <c r="BI24" s="9">
-        <v>2049.0</v>
+        <v>2049</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:61" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>285</v>
       </c>
@@ -5187,7 +5201,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="7">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>65</v>
@@ -5213,10 +5227,10 @@
         <v>72</v>
       </c>
       <c r="O25" s="9">
-        <v>53029.0</v>
+        <v>53029</v>
       </c>
       <c r="P25" s="9">
-        <v>2130.0</v>
+        <v>2130</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>291</v>
@@ -5244,42 +5258,42 @@
       </c>
       <c r="AA25" s="8"/>
       <c r="AB25" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AC25" s="9">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="AD25" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AE25" s="9">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="AF25" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AG25" s="9">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="AH25" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AI25" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AJ25" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AK25" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AL25" s="8"/>
       <c r="AM25" s="8"/>
       <c r="AN25" s="10">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="AO25" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AP25" s="11" t="b">
         <v>0</v>
@@ -5305,7 +5319,7 @@
       </c>
       <c r="AX25" s="13"/>
       <c r="AY25" s="9">
-        <v>14143.0</v>
+        <v>14143</v>
       </c>
       <c r="AZ25" s="7" t="s">
         <v>285</v>
@@ -5332,13 +5346,13 @@
         <v>72</v>
       </c>
       <c r="BH25" s="9">
-        <v>53029.0</v>
+        <v>53029</v>
       </c>
       <c r="BI25" s="9">
-        <v>2130.0</v>
+        <v>2130</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:61" ht="15.75" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>294</v>
       </c>
@@ -5378,10 +5392,10 @@
         <v>72</v>
       </c>
       <c r="O26" s="9">
-        <v>53549.0</v>
+        <v>53549</v>
       </c>
       <c r="P26" s="9">
-        <v>1772.0</v>
+        <v>1772</v>
       </c>
       <c r="Q26" s="8" t="s">
         <v>299</v>
@@ -5409,42 +5423,42 @@
       </c>
       <c r="AA26" s="8"/>
       <c r="AB26" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AC26" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AD26" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AE26" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AF26" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AG26" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AH26" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AI26" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AJ26" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AK26" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AL26" s="8"/>
       <c r="AM26" s="8"/>
       <c r="AN26" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AO26" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AP26" s="11" t="b">
         <v>0</v>
@@ -5470,7 +5484,7 @@
       </c>
       <c r="AX26" s="13"/>
       <c r="AY26" s="9">
-        <v>14154.0</v>
+        <v>14154</v>
       </c>
       <c r="AZ26" s="7" t="s">
         <v>294</v>
@@ -5497,13 +5511,13 @@
         <v>72</v>
       </c>
       <c r="BH26" s="9">
-        <v>53549.0</v>
+        <v>53549</v>
       </c>
       <c r="BI26" s="9">
-        <v>1772.0</v>
+        <v>1772</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:61" ht="15.75" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>302</v>
       </c>
@@ -5541,10 +5555,10 @@
         <v>72</v>
       </c>
       <c r="O27" s="9">
-        <v>53038.0</v>
+        <v>53038</v>
       </c>
       <c r="P27" s="9">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="Q27" s="8" t="s">
         <v>309</v>
@@ -5572,42 +5586,42 @@
       </c>
       <c r="AA27" s="8"/>
       <c r="AB27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AC27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AD27" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AE27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AF27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AG27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AH27" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AI27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AJ27" s="9">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="AK27" s="9">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AL27" s="8"/>
       <c r="AM27" s="8"/>
       <c r="AN27" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AO27" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AP27" s="11" t="b">
         <v>0</v>
@@ -5633,7 +5647,7 @@
       </c>
       <c r="AX27" s="13"/>
       <c r="AY27" s="9">
-        <v>14155.0</v>
+        <v>14155</v>
       </c>
       <c r="AZ27" s="7" t="s">
         <v>302</v>
@@ -5660,13 +5674,13 @@
         <v>72</v>
       </c>
       <c r="BH27" s="9">
-        <v>53038.0</v>
+        <v>53038</v>
       </c>
       <c r="BI27" s="9">
-        <v>130.0</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:61" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>312</v>
       </c>
@@ -5706,10 +5720,10 @@
         <v>72</v>
       </c>
       <c r="O28" s="9">
-        <v>53551.0</v>
+        <v>53551</v>
       </c>
       <c r="P28" s="9">
-        <v>1644.0</v>
+        <v>1644</v>
       </c>
       <c r="Q28" s="8" t="s">
         <v>319</v>
@@ -5737,42 +5751,42 @@
       </c>
       <c r="AA28" s="8"/>
       <c r="AB28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AC28" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AD28" s="9">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AE28" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AF28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AG28" s="9">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="AH28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AI28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AJ28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AK28" s="9">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="AL28" s="8"/>
       <c r="AM28" s="8"/>
       <c r="AN28" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AO28" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="AP28" s="11" t="b">
         <v>0</v>
@@ -5798,7 +5812,7 @@
       </c>
       <c r="AX28" s="13"/>
       <c r="AY28" s="9">
-        <v>14173.0</v>
+        <v>14173</v>
       </c>
       <c r="AZ28" s="7" t="s">
         <v>312</v>
@@ -5825,13 +5839,13 @@
         <v>72</v>
       </c>
       <c r="BH28" s="9">
-        <v>53551.0</v>
+        <v>53551</v>
       </c>
       <c r="BI28" s="9">
-        <v>1644.0</v>
+        <v>1644</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:61" ht="15.75" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>322</v>
       </c>
@@ -5869,10 +5883,10 @@
         <v>72</v>
       </c>
       <c r="O29" s="9">
-        <v>53051.0</v>
+        <v>53051</v>
       </c>
       <c r="P29" s="9">
-        <v>3140.0</v>
+        <v>3140</v>
       </c>
       <c r="Q29" s="8" t="s">
         <v>329</v>
@@ -5900,42 +5914,42 @@
       </c>
       <c r="AA29" s="8"/>
       <c r="AB29" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AC29" s="9">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="AD29" s="9">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="AE29" s="9">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="AF29" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AG29" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AH29" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AI29" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AJ29" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AK29" s="9">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="AL29" s="8"/>
       <c r="AM29" s="8"/>
       <c r="AN29" s="10">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="AO29" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AP29" s="11" t="b">
         <v>0</v>
@@ -5961,7 +5975,7 @@
       </c>
       <c r="AX29" s="13"/>
       <c r="AY29" s="9">
-        <v>14197.0</v>
+        <v>14197</v>
       </c>
       <c r="AZ29" s="7" t="s">
         <v>322</v>
@@ -5988,13 +6002,13 @@
         <v>72</v>
       </c>
       <c r="BH29" s="9">
-        <v>53051.0</v>
+        <v>53051</v>
       </c>
       <c r="BI29" s="9">
-        <v>3140.0</v>
+        <v>3140</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:61" ht="15.75" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>332</v>
       </c>
@@ -6032,10 +6046,10 @@
         <v>72</v>
       </c>
       <c r="O30" s="9">
-        <v>53149.0</v>
+        <v>53149</v>
       </c>
       <c r="P30" s="9">
-        <v>1259.0</v>
+        <v>1259</v>
       </c>
       <c r="Q30" s="8" t="s">
         <v>339</v>
@@ -6063,42 +6077,42 @@
       </c>
       <c r="AA30" s="8"/>
       <c r="AB30" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AC30" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AD30" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AE30" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AF30" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AG30" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AH30" s="9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="AI30" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AJ30" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AK30" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AL30" s="8"/>
       <c r="AM30" s="8"/>
       <c r="AN30" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AO30" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AP30" s="11" t="b">
         <v>0</v>
@@ -6124,7 +6138,7 @@
       </c>
       <c r="AX30" s="13"/>
       <c r="AY30" s="9">
-        <v>14379.0</v>
+        <v>14379</v>
       </c>
       <c r="AZ30" s="7" t="s">
         <v>332</v>
@@ -6151,13 +6165,13 @@
         <v>72</v>
       </c>
       <c r="BH30" s="9">
-        <v>53149.0</v>
+        <v>53149</v>
       </c>
       <c r="BI30" s="9">
-        <v>1259.0</v>
+        <v>1259</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:61" ht="15.75" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>342</v>
       </c>
@@ -6195,10 +6209,10 @@
         <v>72</v>
       </c>
       <c r="O31" s="9">
-        <v>53150.0</v>
+        <v>53150</v>
       </c>
       <c r="P31" s="9">
-        <v>810.0</v>
+        <v>810</v>
       </c>
       <c r="Q31" s="8" t="s">
         <v>348</v>
@@ -6226,42 +6240,42 @@
       </c>
       <c r="AA31" s="8"/>
       <c r="AB31" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AC31" s="9">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="AD31" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AE31" s="9">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AF31" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AG31" s="9">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="AH31" s="9">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="AI31" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AJ31" s="9">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AK31" s="9">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="AL31" s="8"/>
       <c r="AM31" s="8"/>
       <c r="AN31" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="AO31" s="10">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AP31" s="11" t="b">
         <v>0</v>
@@ -6287,7 +6301,7 @@
       </c>
       <c r="AX31" s="13"/>
       <c r="AY31" s="9">
-        <v>14215.0</v>
+        <v>14215</v>
       </c>
       <c r="AZ31" s="7" t="s">
         <v>342</v>
@@ -6314,13 +6328,13 @@
         <v>72</v>
       </c>
       <c r="BH31" s="9">
-        <v>53150.0</v>
+        <v>53150</v>
       </c>
       <c r="BI31" s="9">
-        <v>810.0</v>
+        <v>810</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-worked vrp_solve_07.py to work with procedures in main.py; everything seems to be working up through getting LIBIDs of stops for each route
</commit_message>
<xml_diff>
--- a/hub_recognition_test_data.xlsx
+++ b/hub_recognition_test_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzzlib\PycharmProjects\wilib_vrp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9192297-D3DC-449D-A5BE-55F08023A218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1078,7 +1077,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -1409,20 +1408,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:BI31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AW1" sqref="AW1:AW1048576"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2:AA16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="47" max="47" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="15.75" customHeight="1">
@@ -1681,7 +1680,9 @@
       <c r="Z2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA2" s="8"/>
+      <c r="AA2" s="8">
+        <v>5</v>
+      </c>
       <c r="AB2" s="9">
         <v>4</v>
       </c>
@@ -1840,7 +1841,9 @@
       <c r="Z3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA3" s="8"/>
+      <c r="AA3" s="8">
+        <v>5</v>
+      </c>
       <c r="AB3" s="9">
         <v>1</v>
       </c>
@@ -1977,7 +1980,9 @@
       <c r="Z4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA4" s="8"/>
+      <c r="AA4" s="8">
+        <v>5</v>
+      </c>
       <c r="AB4" s="9">
         <v>6</v>
       </c>
@@ -2140,7 +2145,9 @@
       <c r="Z5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA5" s="8"/>
+      <c r="AA5" s="8">
+        <v>5</v>
+      </c>
       <c r="AB5" s="9">
         <v>1</v>
       </c>
@@ -2263,7 +2270,9 @@
       <c r="Z6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA6" s="8"/>
+      <c r="AA6" s="8">
+        <v>5</v>
+      </c>
       <c r="AB6" s="9">
         <v>1</v>
       </c>
@@ -2388,7 +2397,9 @@
       <c r="Z7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA7" s="8"/>
+      <c r="AA7" s="8">
+        <v>5</v>
+      </c>
       <c r="AB7" s="9">
         <v>2</v>
       </c>
@@ -2551,7 +2562,9 @@
       <c r="Z8" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA8" s="8"/>
+      <c r="AA8" s="8">
+        <v>5</v>
+      </c>
       <c r="AB8" s="9">
         <v>3</v>
       </c>
@@ -2716,7 +2729,9 @@
       <c r="Z9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA9" s="8"/>
+      <c r="AA9" s="8">
+        <v>5</v>
+      </c>
       <c r="AB9" s="9">
         <v>3</v>
       </c>
@@ -2879,7 +2894,9 @@
       <c r="Z10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA10" s="8"/>
+      <c r="AA10" s="8">
+        <v>5</v>
+      </c>
       <c r="AB10" s="9">
         <v>1</v>
       </c>
@@ -3006,7 +3023,9 @@
       <c r="Z11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA11" s="8"/>
+      <c r="AA11" s="8">
+        <v>5</v>
+      </c>
       <c r="AB11" s="9">
         <v>18</v>
       </c>
@@ -3171,7 +3190,9 @@
       <c r="Z12" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA12" s="8"/>
+      <c r="AA12" s="8">
+        <v>5</v>
+      </c>
       <c r="AB12" s="9">
         <v>1</v>
       </c>
@@ -3320,7 +3341,9 @@
       <c r="Z13" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA13" s="8"/>
+      <c r="AA13" s="8">
+        <v>5</v>
+      </c>
       <c r="AB13" s="9">
         <v>1</v>
       </c>
@@ -3487,7 +3510,9 @@
       <c r="Z14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA14" s="8"/>
+      <c r="AA14" s="8">
+        <v>5</v>
+      </c>
       <c r="AB14" s="9">
         <v>4</v>
       </c>
@@ -3652,7 +3677,9 @@
       <c r="Z15" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA15" s="8"/>
+      <c r="AA15" s="8">
+        <v>5</v>
+      </c>
       <c r="AB15" s="9">
         <v>2</v>
       </c>
@@ -3815,7 +3842,9 @@
       <c r="Z16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AA16" s="8"/>
+      <c r="AA16" s="8">
+        <v>5</v>
+      </c>
       <c r="AB16" s="9">
         <v>1</v>
       </c>
@@ -3940,7 +3969,9 @@
       <c r="Z17" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA17" s="8"/>
+      <c r="AA17" s="8">
+        <v>7</v>
+      </c>
       <c r="AB17" s="9">
         <v>2</v>
       </c>
@@ -4107,7 +4138,9 @@
       <c r="Z18" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA18" s="8"/>
+      <c r="AA18" s="8">
+        <v>7</v>
+      </c>
       <c r="AB18" s="9">
         <v>4</v>
       </c>
@@ -4272,7 +4305,9 @@
       <c r="Z19" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA19" s="8"/>
+      <c r="AA19" s="8">
+        <v>7</v>
+      </c>
       <c r="AB19" s="9">
         <v>19</v>
       </c>
@@ -4437,7 +4472,9 @@
       <c r="Z20" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA20" s="8"/>
+      <c r="AA20" s="8">
+        <v>7</v>
+      </c>
       <c r="AB20" s="9">
         <v>4</v>
       </c>
@@ -4600,7 +4637,9 @@
       <c r="Z21" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA21" s="8"/>
+      <c r="AA21" s="8">
+        <v>7</v>
+      </c>
       <c r="AB21" s="9">
         <v>9</v>
       </c>
@@ -4765,7 +4804,9 @@
       <c r="Z22" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA22" s="8"/>
+      <c r="AA22" s="8">
+        <v>7</v>
+      </c>
       <c r="AB22" s="9">
         <v>4</v>
       </c>
@@ -4928,7 +4969,9 @@
       <c r="Z23" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA23" s="8"/>
+      <c r="AA23" s="8">
+        <v>7</v>
+      </c>
       <c r="AB23" s="9">
         <v>7</v>
       </c>
@@ -5091,7 +5134,9 @@
       <c r="Z24" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA24" s="8"/>
+      <c r="AA24" s="8">
+        <v>7</v>
+      </c>
       <c r="AB24" s="9">
         <v>7</v>
       </c>
@@ -5256,7 +5301,9 @@
       <c r="Z25" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA25" s="8"/>
+      <c r="AA25" s="8">
+        <v>7</v>
+      </c>
       <c r="AB25" s="9">
         <v>6</v>
       </c>
@@ -5421,7 +5468,9 @@
       <c r="Z26" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA26" s="8"/>
+      <c r="AA26" s="8">
+        <v>7</v>
+      </c>
       <c r="AB26" s="9">
         <v>3</v>
       </c>
@@ -5584,7 +5633,9 @@
       <c r="Z27" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA27" s="8"/>
+      <c r="AA27" s="8">
+        <v>7</v>
+      </c>
       <c r="AB27" s="9">
         <v>2</v>
       </c>
@@ -5749,7 +5800,9 @@
       <c r="Z28" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA28" s="8"/>
+      <c r="AA28" s="8">
+        <v>7</v>
+      </c>
       <c r="AB28" s="9">
         <v>4</v>
       </c>
@@ -5912,7 +5965,9 @@
       <c r="Z29" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA29" s="8"/>
+      <c r="AA29" s="8">
+        <v>7</v>
+      </c>
       <c r="AB29" s="9">
         <v>10</v>
       </c>
@@ -6075,7 +6130,9 @@
       <c r="Z30" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA30" s="8"/>
+      <c r="AA30" s="8">
+        <v>7</v>
+      </c>
       <c r="AB30" s="9">
         <v>11</v>
       </c>
@@ -6238,7 +6295,9 @@
       <c r="Z31" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AA31" s="8"/>
+      <c r="AA31" s="8">
+        <v>7</v>
+      </c>
       <c r="AB31" s="9">
         <v>9</v>
       </c>

</xml_diff>